<commit_message>
update gudang, pemilihan sales di pengeluaran
</commit_message>
<xml_diff>
--- a/public/DOKUMENTASI/Database.xlsx
+++ b/public/DOKUMENTASI/Database.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\erp-warehouse-vertical\public\DOKUMENTASI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SANDI\erp-warehouse-vertical\public\DOKUMENTASI\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3779C41-568B-4F74-8BCA-2DE878AF3D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="6" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="55">
   <si>
     <t>satuan</t>
   </si>
@@ -193,12 +194,15 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>id_gudang</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -248,7 +252,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 4" xfId="1"/>
+    <cellStyle name="Normal 4" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -339,6 +343,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -374,6 +395,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -549,12 +587,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T97"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -672,7 +708,7 @@
         <v>0</v>
       </c>
       <c r="T3" s="1" t="str">
-        <f t="shared" ref="T3:T65" si="0">$S$2&amp;$R$2&amp;A3</f>
+        <f t="shared" ref="T3:T66" si="0">$S$2&amp;$R$2&amp;A3</f>
         <v>+ tgl_masuk_gudang</v>
       </c>
     </row>
@@ -2836,58 +2872,52 @@
         <v>+ keterangan</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>15</v>
-      </c>
-      <c r="B59" t="s">
+    <row r="59" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="1">
         <v>20</v>
       </c>
-      <c r="D59">
-        <v>0</v>
-      </c>
-      <c r="E59">
-        <v>-1</v>
-      </c>
-      <c r="F59">
-        <v>0</v>
-      </c>
-      <c r="G59">
-        <v>-1</v>
-      </c>
-      <c r="H59">
-        <v>0</v>
-      </c>
-      <c r="I59">
-        <v>0</v>
-      </c>
-      <c r="K59">
-        <v>0</v>
-      </c>
-      <c r="P59">
-        <v>0</v>
-      </c>
-      <c r="Q59">
+      <c r="D59" s="1">
+        <v>0</v>
+      </c>
+      <c r="E59" s="1">
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <v>0</v>
+      </c>
+      <c r="G59" s="1">
+        <v>0</v>
+      </c>
+      <c r="H59" s="1">
+        <v>0</v>
+      </c>
+      <c r="I59" s="1">
+        <v>0</v>
+      </c>
+      <c r="K59" s="1">
         <v>0</v>
       </c>
       <c r="T59" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>+ id_item</v>
+        <v>+ id_gudang</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>15</v>
+      </c>
+      <c r="B60" t="s">
+        <v>4</v>
+      </c>
+      <c r="C60">
         <v>20</v>
       </c>
-      <c r="B60" t="s">
-        <v>21</v>
-      </c>
-      <c r="C60">
-        <v>0</v>
-      </c>
       <c r="D60">
         <v>0</v>
       </c>
@@ -2898,7 +2928,7 @@
         <v>0</v>
       </c>
       <c r="G60">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H60">
         <v>0</v>
@@ -2917,12 +2947,12 @@
       </c>
       <c r="T60" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>+ created_at</v>
+        <v>+ id_item</v>
       </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B61" t="s">
         <v>21</v>
@@ -2959,12 +2989,12 @@
       </c>
       <c r="T61" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>+ updated_at</v>
+        <v>+ created_at</v>
       </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B62" t="s">
         <v>21</v>
@@ -3001,87 +3031,87 @@
       </c>
       <c r="T62" s="1" t="str">
         <f t="shared" si="0"/>
+        <v>+ updated_at</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>23</v>
+      </c>
+      <c r="B63" t="s">
+        <v>21</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>-1</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="K63">
+        <v>0</v>
+      </c>
+      <c r="P63">
+        <v>0</v>
+      </c>
+      <c r="Q63">
+        <v>0</v>
+      </c>
+      <c r="T63" s="1" t="str">
+        <f t="shared" si="0"/>
         <v>+ deleted_at</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="T63" s="1"/>
-    </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
+      <c r="T64" s="1"/>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
-      <c r="J64" s="2"/>
-      <c r="K64" s="2"/>
-      <c r="L64" s="2"/>
-      <c r="M64" s="2"/>
-      <c r="N64" s="2"/>
-      <c r="O64" s="2"/>
-      <c r="P64" s="2"/>
-      <c r="Q64" s="2"/>
-      <c r="R64" s="2"/>
-      <c r="S64" s="2"/>
-      <c r="T64" s="2"/>
-    </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>3</v>
-      </c>
-      <c r="B65" t="s">
-        <v>4</v>
-      </c>
-      <c r="C65">
-        <v>20</v>
-      </c>
-      <c r="D65">
-        <v>0</v>
-      </c>
-      <c r="E65">
-        <v>0</v>
-      </c>
-      <c r="F65">
-        <v>-1</v>
-      </c>
-      <c r="G65">
-        <v>-1</v>
-      </c>
-      <c r="H65">
-        <v>0</v>
-      </c>
-      <c r="I65">
-        <v>0</v>
-      </c>
-      <c r="K65">
-        <v>0</v>
-      </c>
-      <c r="P65">
-        <v>-1</v>
-      </c>
-      <c r="Q65">
-        <v>0</v>
-      </c>
-      <c r="T65" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>+ id</v>
-      </c>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+      <c r="K65" s="2"/>
+      <c r="L65" s="2"/>
+      <c r="M65" s="2"/>
+      <c r="N65" s="2"/>
+      <c r="O65" s="2"/>
+      <c r="P65" s="2"/>
+      <c r="Q65" s="2"/>
+      <c r="R65" s="2"/>
+      <c r="S65" s="2"/>
+      <c r="T65" s="2"/>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="B66" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C66">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -3090,10 +3120,10 @@
         <v>0</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G66">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H66">
         <v>0</v>
@@ -3104,1227 +3134,1270 @@
       <c r="K66">
         <v>0</v>
       </c>
-      <c r="M66" t="s">
-        <v>12</v>
-      </c>
-      <c r="N66" t="s">
-        <v>13</v>
-      </c>
       <c r="P66">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Q66">
         <v>0</v>
       </c>
       <c r="T66" s="1" t="str">
-        <f t="shared" ref="T66:T96" si="1">$S$2&amp;$R$2&amp;A66</f>
-        <v>+ kode_receive</v>
+        <f t="shared" si="0"/>
+        <v>+ id</v>
       </c>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>41</v>
+      </c>
+      <c r="B67" t="s">
+        <v>11</v>
+      </c>
+      <c r="C67">
+        <v>64</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+      <c r="K67">
+        <v>0</v>
+      </c>
+      <c r="M67" t="s">
+        <v>12</v>
+      </c>
+      <c r="N67" t="s">
+        <v>13</v>
+      </c>
+      <c r="P67">
+        <v>0</v>
+      </c>
+      <c r="Q67">
+        <v>0</v>
+      </c>
+      <c r="T67" s="1" t="str">
+        <f t="shared" ref="T67:T97" si="1">$S$2&amp;$R$2&amp;A67</f>
+        <v>+ kode_receive</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>42</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>6</v>
       </c>
-      <c r="C67">
-        <v>0</v>
-      </c>
-      <c r="D67">
-        <v>0</v>
-      </c>
-      <c r="E67">
-        <v>0</v>
-      </c>
-      <c r="F67">
-        <v>0</v>
-      </c>
-      <c r="G67">
-        <v>0</v>
-      </c>
-      <c r="H67">
-        <v>0</v>
-      </c>
-      <c r="I67">
-        <v>0</v>
-      </c>
-      <c r="K67">
-        <v>0</v>
-      </c>
-      <c r="P67">
-        <v>0</v>
-      </c>
-      <c r="Q67">
-        <v>0</v>
-      </c>
-      <c r="T67" s="1" t="str">
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
+      </c>
+      <c r="K68">
+        <v>0</v>
+      </c>
+      <c r="P68">
+        <v>0</v>
+      </c>
+      <c r="Q68">
+        <v>0</v>
+      </c>
+      <c r="T68" s="1" t="str">
         <f t="shared" si="1"/>
         <v>+ tgl_receive</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>28</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B69" t="s">
         <v>11</v>
       </c>
-      <c r="C68">
+      <c r="C69">
         <v>128</v>
       </c>
-      <c r="D68">
-        <v>0</v>
-      </c>
-      <c r="E68">
-        <v>0</v>
-      </c>
-      <c r="F68">
-        <v>0</v>
-      </c>
-      <c r="G68">
-        <v>0</v>
-      </c>
-      <c r="H68">
-        <v>0</v>
-      </c>
-      <c r="I68">
-        <v>0</v>
-      </c>
-      <c r="K68">
-        <v>0</v>
-      </c>
-      <c r="M68" t="s">
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+      <c r="K69">
+        <v>0</v>
+      </c>
+      <c r="M69" t="s">
         <v>12</v>
       </c>
-      <c r="N68" t="s">
+      <c r="N69" t="s">
         <v>13</v>
       </c>
-      <c r="P68">
-        <v>0</v>
-      </c>
-      <c r="Q68">
-        <v>0</v>
-      </c>
-      <c r="T68" s="1" t="str">
+      <c r="P69">
+        <v>0</v>
+      </c>
+      <c r="Q69">
+        <v>0</v>
+      </c>
+      <c r="T69" s="1" t="str">
         <f t="shared" si="1"/>
         <v>+ keterangan</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>33</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B70" t="s">
         <v>11</v>
       </c>
-      <c r="C69">
+      <c r="C70">
         <v>25</v>
       </c>
-      <c r="D69">
-        <v>0</v>
-      </c>
-      <c r="E69">
-        <v>-1</v>
-      </c>
-      <c r="F69">
-        <v>0</v>
-      </c>
-      <c r="G69">
-        <v>0</v>
-      </c>
-      <c r="H69">
-        <v>0</v>
-      </c>
-      <c r="I69">
-        <v>0</v>
-      </c>
-      <c r="K69">
-        <v>0</v>
-      </c>
-      <c r="M69" t="s">
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>-1</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="K70">
+        <v>0</v>
+      </c>
+      <c r="M70" t="s">
         <v>12</v>
       </c>
-      <c r="N69" t="s">
+      <c r="N70" t="s">
         <v>13</v>
       </c>
-      <c r="P69">
-        <v>0</v>
-      </c>
-      <c r="Q69">
-        <v>0</v>
-      </c>
-      <c r="T69" s="1" t="str">
+      <c r="P70">
+        <v>0</v>
+      </c>
+      <c r="Q70">
+        <v>0</v>
+      </c>
+      <c r="T70" s="1" t="str">
         <f t="shared" si="1"/>
         <v>+ status</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>29</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B71" t="s">
         <v>4</v>
       </c>
-      <c r="C70">
+      <c r="C71">
         <v>20</v>
       </c>
-      <c r="D70">
-        <v>0</v>
-      </c>
-      <c r="E70">
-        <v>-1</v>
-      </c>
-      <c r="F70">
-        <v>0</v>
-      </c>
-      <c r="G70">
-        <v>-1</v>
-      </c>
-      <c r="H70">
-        <v>0</v>
-      </c>
-      <c r="I70">
-        <v>0</v>
-      </c>
-      <c r="K70">
-        <v>0</v>
-      </c>
-      <c r="P70">
-        <v>0</v>
-      </c>
-      <c r="Q70">
-        <v>0</v>
-      </c>
-      <c r="T70" s="1" t="str">
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>-1</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>-1</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="K71">
+        <v>0</v>
+      </c>
+      <c r="P71">
+        <v>0</v>
+      </c>
+      <c r="Q71">
+        <v>0</v>
+      </c>
+      <c r="T71" s="1" t="str">
         <f t="shared" si="1"/>
         <v>+ id_user</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>20</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B72" t="s">
         <v>21</v>
       </c>
-      <c r="C71">
-        <v>0</v>
-      </c>
-      <c r="D71">
-        <v>0</v>
-      </c>
-      <c r="E71">
-        <v>-1</v>
-      </c>
-      <c r="F71">
-        <v>0</v>
-      </c>
-      <c r="G71">
-        <v>0</v>
-      </c>
-      <c r="H71">
-        <v>0</v>
-      </c>
-      <c r="I71">
-        <v>0</v>
-      </c>
-      <c r="K71">
-        <v>0</v>
-      </c>
-      <c r="P71">
-        <v>0</v>
-      </c>
-      <c r="Q71">
-        <v>0</v>
-      </c>
-      <c r="T71" s="1" t="str">
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>-1</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="K72">
+        <v>0</v>
+      </c>
+      <c r="P72">
+        <v>0</v>
+      </c>
+      <c r="Q72">
+        <v>0</v>
+      </c>
+      <c r="T72" s="1" t="str">
         <f t="shared" si="1"/>
         <v>+ created_at</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>22</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B73" t="s">
         <v>21</v>
       </c>
-      <c r="C72">
-        <v>0</v>
-      </c>
-      <c r="D72">
-        <v>0</v>
-      </c>
-      <c r="E72">
-        <v>-1</v>
-      </c>
-      <c r="F72">
-        <v>0</v>
-      </c>
-      <c r="G72">
-        <v>0</v>
-      </c>
-      <c r="H72">
-        <v>0</v>
-      </c>
-      <c r="I72">
-        <v>0</v>
-      </c>
-      <c r="K72">
-        <v>0</v>
-      </c>
-      <c r="P72">
-        <v>0</v>
-      </c>
-      <c r="Q72">
-        <v>0</v>
-      </c>
-      <c r="T72" s="1" t="str">
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>-1</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="K73">
+        <v>0</v>
+      </c>
+      <c r="P73">
+        <v>0</v>
+      </c>
+      <c r="Q73">
+        <v>0</v>
+      </c>
+      <c r="T73" s="1" t="str">
         <f t="shared" si="1"/>
         <v>+ updated_at</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>23</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B74" t="s">
         <v>21</v>
       </c>
-      <c r="C73">
-        <v>0</v>
-      </c>
-      <c r="D73">
-        <v>0</v>
-      </c>
-      <c r="E73">
-        <v>-1</v>
-      </c>
-      <c r="F73">
-        <v>0</v>
-      </c>
-      <c r="G73">
-        <v>0</v>
-      </c>
-      <c r="H73">
-        <v>0</v>
-      </c>
-      <c r="I73">
-        <v>0</v>
-      </c>
-      <c r="K73">
-        <v>0</v>
-      </c>
-      <c r="P73">
-        <v>0</v>
-      </c>
-      <c r="Q73">
-        <v>0</v>
-      </c>
-      <c r="T73" s="1" t="str">
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>-1</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+      <c r="I74">
+        <v>0</v>
+      </c>
+      <c r="K74">
+        <v>0</v>
+      </c>
+      <c r="P74">
+        <v>0</v>
+      </c>
+      <c r="Q74">
+        <v>0</v>
+      </c>
+      <c r="T74" s="1" t="str">
         <f t="shared" si="1"/>
         <v>+ deleted_at</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="T74" s="1"/>
-    </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
+      <c r="T75" s="1"/>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
-      <c r="E75" s="2"/>
-      <c r="F75" s="2"/>
-      <c r="G75" s="2"/>
-      <c r="H75" s="2"/>
-      <c r="I75" s="2"/>
-      <c r="J75" s="2"/>
-      <c r="K75" s="2"/>
-      <c r="L75" s="2"/>
-      <c r="M75" s="2"/>
-      <c r="N75" s="2"/>
-      <c r="O75" s="2"/>
-      <c r="P75" s="2"/>
-      <c r="Q75" s="2"/>
-      <c r="R75" s="2"/>
-      <c r="S75" s="2"/>
-      <c r="T75" s="2"/>
-    </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="2"/>
+      <c r="I76" s="2"/>
+      <c r="J76" s="2"/>
+      <c r="K76" s="2"/>
+      <c r="L76" s="2"/>
+      <c r="M76" s="2"/>
+      <c r="N76" s="2"/>
+      <c r="O76" s="2"/>
+      <c r="P76" s="2"/>
+      <c r="Q76" s="2"/>
+      <c r="R76" s="2"/>
+      <c r="S76" s="2"/>
+      <c r="T76" s="2"/>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>3</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B77" t="s">
         <v>4</v>
       </c>
-      <c r="C76">
+      <c r="C77">
         <v>20</v>
       </c>
-      <c r="D76">
-        <v>0</v>
-      </c>
-      <c r="E76">
-        <v>0</v>
-      </c>
-      <c r="F76">
-        <v>-1</v>
-      </c>
-      <c r="G76">
-        <v>-1</v>
-      </c>
-      <c r="H76">
-        <v>0</v>
-      </c>
-      <c r="I76">
-        <v>0</v>
-      </c>
-      <c r="K76">
-        <v>0</v>
-      </c>
-      <c r="P76">
-        <v>-1</v>
-      </c>
-      <c r="Q76">
-        <v>0</v>
-      </c>
-      <c r="T76" s="1" t="str">
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <v>-1</v>
+      </c>
+      <c r="G77">
+        <v>-1</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
+      </c>
+      <c r="K77">
+        <v>0</v>
+      </c>
+      <c r="P77">
+        <v>-1</v>
+      </c>
+      <c r="Q77">
+        <v>0</v>
+      </c>
+      <c r="T77" s="1" t="str">
         <f t="shared" si="1"/>
         <v>+ id</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>16</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B78" t="s">
         <v>4</v>
       </c>
-      <c r="C77">
+      <c r="C78">
         <v>20</v>
       </c>
-      <c r="D77">
-        <v>0</v>
-      </c>
-      <c r="E77">
-        <v>-1</v>
-      </c>
-      <c r="F77">
-        <v>0</v>
-      </c>
-      <c r="G77">
-        <v>-1</v>
-      </c>
-      <c r="H77">
-        <v>0</v>
-      </c>
-      <c r="I77">
-        <v>0</v>
-      </c>
-      <c r="K77">
-        <v>0</v>
-      </c>
-      <c r="P77">
-        <v>0</v>
-      </c>
-      <c r="Q77">
-        <v>0</v>
-      </c>
-      <c r="T77" s="1" t="str">
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78">
+        <v>-1</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <v>-1</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
+      <c r="I78">
+        <v>0</v>
+      </c>
+      <c r="K78">
+        <v>0</v>
+      </c>
+      <c r="P78">
+        <v>0</v>
+      </c>
+      <c r="Q78">
+        <v>0</v>
+      </c>
+      <c r="T78" s="1" t="str">
         <f t="shared" si="1"/>
         <v>+ id_receive</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>15</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B79" t="s">
         <v>4</v>
       </c>
-      <c r="C78">
+      <c r="C79">
         <v>20</v>
       </c>
-      <c r="D78">
-        <v>0</v>
-      </c>
-      <c r="E78">
-        <v>-1</v>
-      </c>
-      <c r="F78">
-        <v>0</v>
-      </c>
-      <c r="G78">
-        <v>-1</v>
-      </c>
-      <c r="H78">
-        <v>0</v>
-      </c>
-      <c r="I78">
-        <v>0</v>
-      </c>
-      <c r="K78">
-        <v>0</v>
-      </c>
-      <c r="P78">
-        <v>0</v>
-      </c>
-      <c r="Q78">
-        <v>0</v>
-      </c>
-      <c r="T78" s="1" t="str">
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <v>-1</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>-1</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+      <c r="I79">
+        <v>0</v>
+      </c>
+      <c r="K79">
+        <v>0</v>
+      </c>
+      <c r="P79">
+        <v>0</v>
+      </c>
+      <c r="Q79">
+        <v>0</v>
+      </c>
+      <c r="T79" s="1" t="str">
         <f t="shared" si="1"/>
         <v>+ id_item</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>7</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B80" t="s">
         <v>8</v>
       </c>
-      <c r="C79">
-        <v>0</v>
-      </c>
-      <c r="D79">
-        <v>0</v>
-      </c>
-      <c r="E79">
-        <v>-1</v>
-      </c>
-      <c r="F79">
-        <v>0</v>
-      </c>
-      <c r="G79">
-        <v>0</v>
-      </c>
-      <c r="H79">
-        <v>0</v>
-      </c>
-      <c r="I79">
-        <v>0</v>
-      </c>
-      <c r="K79">
-        <v>0</v>
-      </c>
-      <c r="P79">
-        <v>0</v>
-      </c>
-      <c r="Q79">
-        <v>0</v>
-      </c>
-      <c r="T79" s="1" t="str">
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>-1</v>
+      </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+      <c r="I80">
+        <v>0</v>
+      </c>
+      <c r="K80">
+        <v>0</v>
+      </c>
+      <c r="P80">
+        <v>0</v>
+      </c>
+      <c r="Q80">
+        <v>0</v>
+      </c>
+      <c r="T80" s="1" t="str">
         <f t="shared" si="1"/>
         <v>+ qty</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>20</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B81" t="s">
         <v>21</v>
       </c>
-      <c r="C80">
-        <v>0</v>
-      </c>
-      <c r="D80">
-        <v>0</v>
-      </c>
-      <c r="E80">
-        <v>-1</v>
-      </c>
-      <c r="F80">
-        <v>0</v>
-      </c>
-      <c r="G80">
-        <v>0</v>
-      </c>
-      <c r="H80">
-        <v>0</v>
-      </c>
-      <c r="I80">
-        <v>0</v>
-      </c>
-      <c r="K80">
-        <v>0</v>
-      </c>
-      <c r="P80">
-        <v>0</v>
-      </c>
-      <c r="Q80">
-        <v>0</v>
-      </c>
-      <c r="T80" s="1" t="str">
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <v>-1</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+      <c r="I81">
+        <v>0</v>
+      </c>
+      <c r="K81">
+        <v>0</v>
+      </c>
+      <c r="P81">
+        <v>0</v>
+      </c>
+      <c r="Q81">
+        <v>0</v>
+      </c>
+      <c r="T81" s="1" t="str">
         <f t="shared" si="1"/>
         <v>+ created_at</v>
       </c>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>22</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B82" t="s">
         <v>21</v>
       </c>
-      <c r="C81">
-        <v>0</v>
-      </c>
-      <c r="D81">
-        <v>0</v>
-      </c>
-      <c r="E81">
-        <v>-1</v>
-      </c>
-      <c r="F81">
-        <v>0</v>
-      </c>
-      <c r="G81">
-        <v>0</v>
-      </c>
-      <c r="H81">
-        <v>0</v>
-      </c>
-      <c r="I81">
-        <v>0</v>
-      </c>
-      <c r="K81">
-        <v>0</v>
-      </c>
-      <c r="P81">
-        <v>0</v>
-      </c>
-      <c r="Q81">
-        <v>0</v>
-      </c>
-      <c r="T81" s="1" t="str">
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>-1</v>
+      </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+      <c r="I82">
+        <v>0</v>
+      </c>
+      <c r="K82">
+        <v>0</v>
+      </c>
+      <c r="P82">
+        <v>0</v>
+      </c>
+      <c r="Q82">
+        <v>0</v>
+      </c>
+      <c r="T82" s="1" t="str">
         <f t="shared" si="1"/>
         <v>+ updated_at</v>
       </c>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>23</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B83" t="s">
         <v>21</v>
       </c>
-      <c r="C82">
-        <v>0</v>
-      </c>
-      <c r="D82">
-        <v>0</v>
-      </c>
-      <c r="E82">
-        <v>-1</v>
-      </c>
-      <c r="F82">
-        <v>0</v>
-      </c>
-      <c r="G82">
-        <v>0</v>
-      </c>
-      <c r="H82">
-        <v>0</v>
-      </c>
-      <c r="I82">
-        <v>0</v>
-      </c>
-      <c r="K82">
-        <v>0</v>
-      </c>
-      <c r="P82">
-        <v>0</v>
-      </c>
-      <c r="Q82">
-        <v>0</v>
-      </c>
-      <c r="T82" s="1" t="str">
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>-1</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+      <c r="H83">
+        <v>0</v>
+      </c>
+      <c r="I83">
+        <v>0</v>
+      </c>
+      <c r="K83">
+        <v>0</v>
+      </c>
+      <c r="P83">
+        <v>0</v>
+      </c>
+      <c r="Q83">
+        <v>0</v>
+      </c>
+      <c r="T83" s="1" t="str">
         <f t="shared" si="1"/>
         <v>+ deleted_at</v>
       </c>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="T83" s="1"/>
-    </row>
     <row r="84" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
+      <c r="T84" s="1"/>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B84" s="2"/>
-      <c r="C84" s="2"/>
-      <c r="D84" s="2"/>
-      <c r="E84" s="2"/>
-      <c r="F84" s="2"/>
-      <c r="G84" s="2"/>
-      <c r="H84" s="2"/>
-      <c r="I84" s="2"/>
-      <c r="J84" s="2"/>
-      <c r="K84" s="2"/>
-      <c r="L84" s="2"/>
-      <c r="M84" s="2"/>
-      <c r="N84" s="2"/>
-      <c r="O84" s="2"/>
-      <c r="P84" s="2"/>
-      <c r="Q84" s="2"/>
-      <c r="R84" s="2"/>
-      <c r="S84" s="2"/>
-      <c r="T84" s="2"/>
-    </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+      <c r="B85" s="2"/>
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+      <c r="G85" s="2"/>
+      <c r="H85" s="2"/>
+      <c r="I85" s="2"/>
+      <c r="J85" s="2"/>
+      <c r="K85" s="2"/>
+      <c r="L85" s="2"/>
+      <c r="M85" s="2"/>
+      <c r="N85" s="2"/>
+      <c r="O85" s="2"/>
+      <c r="P85" s="2"/>
+      <c r="Q85" s="2"/>
+      <c r="R85" s="2"/>
+      <c r="S85" s="2"/>
+      <c r="T85" s="2"/>
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>3</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B86" t="s">
         <v>4</v>
       </c>
-      <c r="C85">
+      <c r="C86">
         <v>20</v>
       </c>
-      <c r="D85">
-        <v>0</v>
-      </c>
-      <c r="E85">
-        <v>0</v>
-      </c>
-      <c r="F85">
-        <v>-1</v>
-      </c>
-      <c r="G85">
-        <v>-1</v>
-      </c>
-      <c r="H85">
-        <v>0</v>
-      </c>
-      <c r="I85">
-        <v>0</v>
-      </c>
-      <c r="K85">
-        <v>0</v>
-      </c>
-      <c r="P85">
-        <v>-1</v>
-      </c>
-      <c r="Q85">
-        <v>0</v>
-      </c>
-      <c r="T85" s="1" t="str">
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="F86">
+        <v>-1</v>
+      </c>
+      <c r="G86">
+        <v>-1</v>
+      </c>
+      <c r="H86">
+        <v>0</v>
+      </c>
+      <c r="I86">
+        <v>0</v>
+      </c>
+      <c r="K86">
+        <v>0</v>
+      </c>
+      <c r="P86">
+        <v>-1</v>
+      </c>
+      <c r="Q86">
+        <v>0</v>
+      </c>
+      <c r="T86" s="1" t="str">
         <f t="shared" si="1"/>
         <v>+ id</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>45</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B87" t="s">
         <v>11</v>
       </c>
-      <c r="C86">
+      <c r="C87">
         <v>255</v>
       </c>
-      <c r="D86">
-        <v>0</v>
-      </c>
-      <c r="E86">
-        <v>0</v>
-      </c>
-      <c r="F86">
-        <v>0</v>
-      </c>
-      <c r="G86">
-        <v>0</v>
-      </c>
-      <c r="H86">
-        <v>0</v>
-      </c>
-      <c r="I86">
-        <v>0</v>
-      </c>
-      <c r="K86">
-        <v>0</v>
-      </c>
-      <c r="M86" t="s">
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87">
+        <v>0</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+      <c r="H87">
+        <v>0</v>
+      </c>
+      <c r="I87">
+        <v>0</v>
+      </c>
+      <c r="K87">
+        <v>0</v>
+      </c>
+      <c r="M87" t="s">
         <v>12</v>
       </c>
-      <c r="N86" t="s">
+      <c r="N87" t="s">
         <v>13</v>
       </c>
-      <c r="P86">
-        <v>0</v>
-      </c>
-      <c r="Q86">
-        <v>0</v>
-      </c>
-      <c r="T86" s="1" t="str">
+      <c r="P87">
+        <v>0</v>
+      </c>
+      <c r="Q87">
+        <v>0</v>
+      </c>
+      <c r="T87" s="1" t="str">
         <f t="shared" si="1"/>
         <v>+ name</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>46</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B88" t="s">
         <v>11</v>
       </c>
-      <c r="C87">
+      <c r="C88">
         <v>255</v>
       </c>
-      <c r="D87">
-        <v>0</v>
-      </c>
-      <c r="E87">
-        <v>0</v>
-      </c>
-      <c r="F87">
-        <v>0</v>
-      </c>
-      <c r="G87">
-        <v>0</v>
-      </c>
-      <c r="H87">
-        <v>0</v>
-      </c>
-      <c r="I87">
-        <v>0</v>
-      </c>
-      <c r="K87">
-        <v>0</v>
-      </c>
-      <c r="M87" t="s">
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>0</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
+      </c>
+      <c r="I88">
+        <v>0</v>
+      </c>
+      <c r="K88">
+        <v>0</v>
+      </c>
+      <c r="M88" t="s">
         <v>12</v>
       </c>
-      <c r="N87" t="s">
+      <c r="N88" t="s">
         <v>13</v>
       </c>
-      <c r="P87">
-        <v>0</v>
-      </c>
-      <c r="Q87">
-        <v>0</v>
-      </c>
-      <c r="T87" s="1" t="str">
+      <c r="P88">
+        <v>0</v>
+      </c>
+      <c r="Q88">
+        <v>0</v>
+      </c>
+      <c r="T88" s="1" t="str">
         <f t="shared" si="1"/>
         <v>+ email</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>47</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B89" t="s">
         <v>21</v>
       </c>
-      <c r="C88">
-        <v>0</v>
-      </c>
-      <c r="D88">
-        <v>0</v>
-      </c>
-      <c r="E88">
-        <v>-1</v>
-      </c>
-      <c r="F88">
-        <v>0</v>
-      </c>
-      <c r="G88">
-        <v>0</v>
-      </c>
-      <c r="H88">
-        <v>0</v>
-      </c>
-      <c r="I88">
-        <v>0</v>
-      </c>
-      <c r="K88">
-        <v>0</v>
-      </c>
-      <c r="P88">
-        <v>0</v>
-      </c>
-      <c r="Q88">
-        <v>0</v>
-      </c>
-      <c r="T88" s="1" t="str">
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="E89">
+        <v>-1</v>
+      </c>
+      <c r="F89">
+        <v>0</v>
+      </c>
+      <c r="G89">
+        <v>0</v>
+      </c>
+      <c r="H89">
+        <v>0</v>
+      </c>
+      <c r="I89">
+        <v>0</v>
+      </c>
+      <c r="K89">
+        <v>0</v>
+      </c>
+      <c r="P89">
+        <v>0</v>
+      </c>
+      <c r="Q89">
+        <v>0</v>
+      </c>
+      <c r="T89" s="1" t="str">
         <f t="shared" si="1"/>
         <v>+ email_verified_at</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>48</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B90" t="s">
         <v>11</v>
       </c>
-      <c r="C89">
+      <c r="C90">
         <v>255</v>
       </c>
-      <c r="D89">
-        <v>0</v>
-      </c>
-      <c r="E89">
-        <v>0</v>
-      </c>
-      <c r="F89">
-        <v>0</v>
-      </c>
-      <c r="G89">
-        <v>0</v>
-      </c>
-      <c r="H89">
-        <v>0</v>
-      </c>
-      <c r="I89">
-        <v>0</v>
-      </c>
-      <c r="K89">
-        <v>0</v>
-      </c>
-      <c r="M89" t="s">
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="F90">
+        <v>0</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
+      <c r="I90">
+        <v>0</v>
+      </c>
+      <c r="K90">
+        <v>0</v>
+      </c>
+      <c r="M90" t="s">
         <v>12</v>
       </c>
-      <c r="N89" t="s">
+      <c r="N90" t="s">
         <v>13</v>
       </c>
-      <c r="P89">
-        <v>0</v>
-      </c>
-      <c r="Q89">
-        <v>0</v>
-      </c>
-      <c r="T89" s="1" t="str">
+      <c r="P90">
+        <v>0</v>
+      </c>
+      <c r="Q90">
+        <v>0</v>
+      </c>
+      <c r="T90" s="1" t="str">
         <f t="shared" si="1"/>
         <v>+ password</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>49</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B91" t="s">
         <v>11</v>
       </c>
-      <c r="C90">
+      <c r="C91">
         <v>255</v>
       </c>
-      <c r="D90">
-        <v>0</v>
-      </c>
-      <c r="E90">
-        <v>0</v>
-      </c>
-      <c r="F90">
-        <v>0</v>
-      </c>
-      <c r="G90">
-        <v>0</v>
-      </c>
-      <c r="H90">
-        <v>0</v>
-      </c>
-      <c r="I90">
-        <v>0</v>
-      </c>
-      <c r="K90">
-        <v>0</v>
-      </c>
-      <c r="M90" t="s">
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+      <c r="F91">
+        <v>0</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+      <c r="H91">
+        <v>0</v>
+      </c>
+      <c r="I91">
+        <v>0</v>
+      </c>
+      <c r="K91">
+        <v>0</v>
+      </c>
+      <c r="M91" t="s">
         <v>12</v>
       </c>
-      <c r="N90" t="s">
+      <c r="N91" t="s">
         <v>13</v>
       </c>
-      <c r="P90">
-        <v>0</v>
-      </c>
-      <c r="Q90">
-        <v>0</v>
-      </c>
-      <c r="T90" s="1" t="str">
+      <c r="P91">
+        <v>0</v>
+      </c>
+      <c r="Q91">
+        <v>0</v>
+      </c>
+      <c r="T91" s="1" t="str">
         <f t="shared" si="1"/>
         <v>+ roles</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>33</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B92" t="s">
         <v>11</v>
       </c>
-      <c r="C91">
+      <c r="C92">
         <v>255</v>
       </c>
-      <c r="D91">
-        <v>0</v>
-      </c>
-      <c r="E91">
-        <v>0</v>
-      </c>
-      <c r="F91">
-        <v>0</v>
-      </c>
-      <c r="G91">
-        <v>0</v>
-      </c>
-      <c r="H91">
-        <v>0</v>
-      </c>
-      <c r="I91">
-        <v>0</v>
-      </c>
-      <c r="K91">
-        <v>0</v>
-      </c>
-      <c r="M91" t="s">
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="E92">
+        <v>0</v>
+      </c>
+      <c r="F92">
+        <v>0</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
+      <c r="I92">
+        <v>0</v>
+      </c>
+      <c r="K92">
+        <v>0</v>
+      </c>
+      <c r="M92" t="s">
         <v>12</v>
       </c>
-      <c r="N91" t="s">
+      <c r="N92" t="s">
         <v>13</v>
       </c>
-      <c r="P91">
-        <v>0</v>
-      </c>
-      <c r="Q91">
-        <v>0</v>
-      </c>
-      <c r="T91" s="1" t="str">
+      <c r="P92">
+        <v>0</v>
+      </c>
+      <c r="Q92">
+        <v>0</v>
+      </c>
+      <c r="T92" s="1" t="str">
         <f t="shared" si="1"/>
         <v>+ status</v>
       </c>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>50</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B93" t="s">
         <v>11</v>
       </c>
-      <c r="C92">
+      <c r="C93">
         <v>64</v>
       </c>
-      <c r="D92">
-        <v>0</v>
-      </c>
-      <c r="E92">
-        <v>-1</v>
-      </c>
-      <c r="F92">
-        <v>0</v>
-      </c>
-      <c r="G92">
-        <v>0</v>
-      </c>
-      <c r="H92">
-        <v>0</v>
-      </c>
-      <c r="I92">
-        <v>0</v>
-      </c>
-      <c r="K92">
-        <v>0</v>
-      </c>
-      <c r="M92" t="s">
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>-1</v>
+      </c>
+      <c r="F93">
+        <v>0</v>
+      </c>
+      <c r="G93">
+        <v>0</v>
+      </c>
+      <c r="H93">
+        <v>0</v>
+      </c>
+      <c r="I93">
+        <v>0</v>
+      </c>
+      <c r="K93">
+        <v>0</v>
+      </c>
+      <c r="M93" t="s">
         <v>12</v>
       </c>
-      <c r="N92" t="s">
+      <c r="N93" t="s">
         <v>13</v>
       </c>
-      <c r="P92">
-        <v>0</v>
-      </c>
-      <c r="Q92">
-        <v>0</v>
-      </c>
-      <c r="T92" s="1" t="str">
+      <c r="P93">
+        <v>0</v>
+      </c>
+      <c r="Q93">
+        <v>0</v>
+      </c>
+      <c r="T93" s="1" t="str">
         <f t="shared" si="1"/>
         <v>+ foto</v>
       </c>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>51</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B94" t="s">
         <v>11</v>
       </c>
-      <c r="C93">
+      <c r="C94">
         <v>100</v>
       </c>
-      <c r="D93">
-        <v>0</v>
-      </c>
-      <c r="E93">
-        <v>-1</v>
-      </c>
-      <c r="F93">
-        <v>0</v>
-      </c>
-      <c r="G93">
-        <v>0</v>
-      </c>
-      <c r="H93">
-        <v>0</v>
-      </c>
-      <c r="I93">
-        <v>0</v>
-      </c>
-      <c r="K93">
-        <v>0</v>
-      </c>
-      <c r="M93" t="s">
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94">
+        <v>-1</v>
+      </c>
+      <c r="F94">
+        <v>0</v>
+      </c>
+      <c r="G94">
+        <v>0</v>
+      </c>
+      <c r="H94">
+        <v>0</v>
+      </c>
+      <c r="I94">
+        <v>0</v>
+      </c>
+      <c r="K94">
+        <v>0</v>
+      </c>
+      <c r="M94" t="s">
         <v>12</v>
       </c>
-      <c r="N93" t="s">
+      <c r="N94" t="s">
         <v>13</v>
       </c>
-      <c r="P93">
-        <v>0</v>
-      </c>
-      <c r="Q93">
-        <v>0</v>
-      </c>
-      <c r="T93" s="1" t="str">
+      <c r="P94">
+        <v>0</v>
+      </c>
+      <c r="Q94">
+        <v>0</v>
+      </c>
+      <c r="T94" s="1" t="str">
         <f t="shared" si="1"/>
         <v>+ remember_token</v>
       </c>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>20</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B95" t="s">
         <v>21</v>
       </c>
-      <c r="C94">
-        <v>0</v>
-      </c>
-      <c r="D94">
-        <v>0</v>
-      </c>
-      <c r="E94">
-        <v>-1</v>
-      </c>
-      <c r="F94">
-        <v>0</v>
-      </c>
-      <c r="G94">
-        <v>0</v>
-      </c>
-      <c r="H94">
-        <v>0</v>
-      </c>
-      <c r="I94">
-        <v>0</v>
-      </c>
-      <c r="K94">
-        <v>0</v>
-      </c>
-      <c r="P94">
-        <v>0</v>
-      </c>
-      <c r="Q94">
-        <v>0</v>
-      </c>
-      <c r="T94" s="1" t="str">
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95">
+        <v>-1</v>
+      </c>
+      <c r="F95">
+        <v>0</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95">
+        <v>0</v>
+      </c>
+      <c r="K95">
+        <v>0</v>
+      </c>
+      <c r="P95">
+        <v>0</v>
+      </c>
+      <c r="Q95">
+        <v>0</v>
+      </c>
+      <c r="T95" s="1" t="str">
         <f t="shared" si="1"/>
         <v>+ created_at</v>
       </c>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>22</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B96" t="s">
         <v>21</v>
       </c>
-      <c r="C95">
-        <v>0</v>
-      </c>
-      <c r="D95">
-        <v>0</v>
-      </c>
-      <c r="E95">
-        <v>-1</v>
-      </c>
-      <c r="F95">
-        <v>0</v>
-      </c>
-      <c r="G95">
-        <v>0</v>
-      </c>
-      <c r="H95">
-        <v>0</v>
-      </c>
-      <c r="I95">
-        <v>0</v>
-      </c>
-      <c r="K95">
-        <v>0</v>
-      </c>
-      <c r="P95">
-        <v>0</v>
-      </c>
-      <c r="Q95">
-        <v>0</v>
-      </c>
-      <c r="T95" s="1" t="str">
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96">
+        <v>-1</v>
+      </c>
+      <c r="F96">
+        <v>0</v>
+      </c>
+      <c r="G96">
+        <v>0</v>
+      </c>
+      <c r="H96">
+        <v>0</v>
+      </c>
+      <c r="I96">
+        <v>0</v>
+      </c>
+      <c r="K96">
+        <v>0</v>
+      </c>
+      <c r="P96">
+        <v>0</v>
+      </c>
+      <c r="Q96">
+        <v>0</v>
+      </c>
+      <c r="T96" s="1" t="str">
         <f t="shared" si="1"/>
         <v>+ updated_at</v>
       </c>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>23</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B97" t="s">
         <v>21</v>
       </c>
-      <c r="C96">
-        <v>0</v>
-      </c>
-      <c r="D96">
-        <v>0</v>
-      </c>
-      <c r="E96">
-        <v>-1</v>
-      </c>
-      <c r="F96">
-        <v>0</v>
-      </c>
-      <c r="G96">
-        <v>0</v>
-      </c>
-      <c r="H96">
-        <v>0</v>
-      </c>
-      <c r="I96">
-        <v>0</v>
-      </c>
-      <c r="K96">
-        <v>0</v>
-      </c>
-      <c r="P96">
-        <v>0</v>
-      </c>
-      <c r="Q96">
-        <v>0</v>
-      </c>
-      <c r="T96" s="1" t="str">
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>-1</v>
+      </c>
+      <c r="F97">
+        <v>0</v>
+      </c>
+      <c r="G97">
+        <v>0</v>
+      </c>
+      <c r="H97">
+        <v>0</v>
+      </c>
+      <c r="I97">
+        <v>0</v>
+      </c>
+      <c r="K97">
+        <v>0</v>
+      </c>
+      <c r="P97">
+        <v>0</v>
+      </c>
+      <c r="Q97">
+        <v>0</v>
+      </c>
+      <c r="T97" s="1" t="str">
         <f t="shared" si="1"/>
         <v>+ deleted_at</v>
       </c>
     </row>
-    <row r="97" spans="20:20" x14ac:dyDescent="0.25">
-      <c r="T97" s="1"/>
+    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T98" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>